<commit_message>
Add more data to game performance experiment.
</commit_message>
<xml_diff>
--- a/tex/evaluation/resources/performance/data.xlsx
+++ b/tex/evaluation/resources/performance/data.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braden\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\University\Computer Science\Modules\CM3203\Project\report\tex\evaluation\resources\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17400" windowHeight="8655" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17400" windowHeight="8655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="76" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +55,7 @@
     <t>Column Labels</t>
   </si>
   <si>
-    <t>Update Duration</t>
+    <t>Sum of duration</t>
   </si>
 </sst>
 </file>
@@ -107,13 +107,13 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -145,44 +145,39 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Book1.xlsx]Summary!PivotTable5</c:name>
+    <c:name>[daata.xlsx]Summary!PivotTable5</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
@@ -202,6 +197,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -215,11 +213,11 @@
           <c:size val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln w="9525">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -229,6 +227,9 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -299,6 +300,87 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -343,25 +425,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Summary!$A$5:$A$11</c:f>
@@ -395,22 +458,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.39859999999607643</c:v>
+                  <c:v>1.992999999980382</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48080000000190859</c:v>
+                  <c:v>2.4040000000095429</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54400000000023252</c:v>
+                  <c:v>2.7200000000011624</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61200000000026145</c:v>
+                  <c:v>3.060000000001307</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63680000000022063</c:v>
+                  <c:v>3.1840000000011033</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.81360000000131516</c:v>
+                  <c:v>4.0680000000065757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,7 +481,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-35DE-487F-92E1-200999458168}"/>
+              <c16:uniqueId val="{00000001-6C27-49E2-961E-3591F8431A90}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -431,7 +494,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -460,25 +523,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Summary!$A$5:$A$11</c:f>
@@ -512,22 +556,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.45599999999976698</c:v>
+                  <c:v>2.1340000000054689</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47979999999806699</c:v>
+                  <c:v>2.5550000000039259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65060000000230445</c:v>
+                  <c:v>4.5459999999991672</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0149999999994148</c:v>
+                  <c:v>4.1219999999957491</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2330000000074459</c:v>
+                  <c:v>5.5139999999955567</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4508000000030701</c:v>
+                  <c:v>5.8519999999843861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,7 +579,301 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-35DE-487F-92E1-200999458168}"/>
+              <c16:uniqueId val="{00000005-6C27-49E2-961E-3591F8431A90}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$D$5:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.164999999997232</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.566999999995458</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.809999999997669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0300000000133824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0119999999878759</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9089999999850695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-6C27-49E2-961E-3591F8431A90}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>750</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$E$5:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.5640000000003043</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2960000000057308</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4330000000016279</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1880000000091933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0320000000064997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7840000000287199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E084-4DB3-89CB-4598E889FCFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$F$5:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.279999999998835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3989999999903349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.253000000011522</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0749999999970745</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1650000000372298</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2540000000153499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E084-4DB3-89CB-4598E889FCFC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1435,16 +1773,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1473,7 +1811,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Braden Marshall" refreshedDate="42856.084087499999" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Braden Marshall" refreshedDate="42857.055542824077" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="150">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -1489,74 +1827,16 @@
       </sharedItems>
     </cacheField>
     <cacheField name="starttime" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1000" count="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1000" count="5">
         <n v="0"/>
+        <n v="250"/>
+        <n v="500"/>
+        <n v="750"/>
         <n v="1000"/>
       </sharedItems>
     </cacheField>
     <cacheField name="duration" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.331999999994877" maxValue="1.6530000000056999" count="60">
-        <n v="0.42100000000209498"/>
-        <n v="0.48899999999412103"/>
-        <n v="0.37799999999697298"/>
-        <n v="0.331999999994877"/>
-        <n v="0.37299999999231598"/>
-        <n v="0.46400000000721697"/>
-        <n v="0.45600000000013002"/>
-        <n v="0.46500000000014502"/>
-        <n v="0.60900000000037802"/>
-        <n v="0.41000000000167303"/>
-        <n v="0.43900000000212402"/>
-        <n v="0.58399999999892305"/>
-        <n v="0.48400000000037802"/>
-        <n v="0.46099999999933"/>
-        <n v="0.75200000000040701"/>
-        <n v="0.55199999999967897"/>
-        <n v="0.68999999999868999"/>
-        <n v="0.69800000000032003"/>
-        <n v="0.60800000000017396"/>
-        <n v="0.51200000000244394"/>
-        <n v="0.60700000000360799"/>
-        <n v="0.62299999999959199"/>
-        <n v="0.72899999999935905"/>
-        <n v="0.60399999999935905"/>
-        <n v="0.62099999999918498"/>
-        <n v="0.93400000000110595"/>
-        <n v="0.69700000000011597"/>
-        <n v="0.94800000000395801"/>
-        <n v="0.77000000000407398"/>
-        <n v="0.718999999997322"/>
-        <n v="0.44399999999950501"/>
-        <n v="0.46700000000055297"/>
-        <n v="0.42499999999927202"/>
-        <n v="0.43699999999807898"/>
-        <n v="0.50700000000142598"/>
-        <n v="0.51899999999295598"/>
-        <n v="0.42499999999563398"/>
-        <n v="0.58299999999871899"/>
-        <n v="0.37600000000384098"/>
-        <n v="0.49599999999918498"/>
-        <n v="0.69600000000355"/>
-        <n v="0.70200000000477303"/>
-        <n v="0.703000000001338"/>
-        <n v="0.61100000000442301"/>
-        <n v="0.54099999999743797"/>
-        <n v="1.12400000000343"/>
-        <n v="1.4530000000013299"/>
-        <n v="0.84600000000500497"/>
-        <n v="0.788000000000465"/>
-        <n v="0.86399999998684496"/>
-        <n v="1.16199999995296"/>
-        <n v="1.2820000000065099"/>
-        <n v="1.24900000001071"/>
-        <n v="1.1330000000307301"/>
-        <n v="1.33900000003632"/>
-        <n v="1.6530000000056999"/>
-        <n v="1.20999999999185"/>
-        <n v="1.3739999999961501"/>
-        <n v="1.6000000000058201"/>
-        <n v="1.41700000001583"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.331999999994877" maxValue="2.7630000000062802"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1568,313 +1848,763 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="60">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="150">
   <r>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="0.42100000000209498"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="0.48899999999412103"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="0.37799999999697298"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="0.331999999994877"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="0.37299999999231598"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="0.46400000000721697"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="0.45600000000013002"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="7"/>
+    <n v="0.46500000000014502"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="8"/>
+    <n v="0.60900000000037802"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="9"/>
+    <n v="0.41000000000167303"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
-    <x v="10"/>
+    <n v="0.43900000000212402"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
-    <x v="11"/>
+    <n v="0.58399999999892305"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
-    <x v="12"/>
+    <n v="0.48400000000037802"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
-    <x v="13"/>
+    <n v="0.46099999999933"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
-    <x v="14"/>
+    <n v="0.75200000000040701"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
-    <x v="15"/>
+    <n v="0.55199999999967897"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
-    <x v="16"/>
+    <n v="0.68999999999868999"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
-    <x v="17"/>
+    <n v="0.69800000000032003"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
-    <x v="18"/>
+    <n v="0.60800000000017396"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
-    <x v="19"/>
+    <n v="0.51200000000244394"/>
   </r>
   <r>
     <x v="4"/>
     <x v="0"/>
-    <x v="20"/>
+    <n v="0.60700000000360799"/>
   </r>
   <r>
     <x v="4"/>
     <x v="0"/>
-    <x v="21"/>
+    <n v="0.62299999999959199"/>
   </r>
   <r>
     <x v="4"/>
     <x v="0"/>
-    <x v="22"/>
+    <n v="0.72899999999935905"/>
   </r>
   <r>
     <x v="4"/>
     <x v="0"/>
-    <x v="23"/>
+    <n v="0.60399999999935905"/>
   </r>
   <r>
     <x v="4"/>
     <x v="0"/>
-    <x v="24"/>
+    <n v="0.62099999999918498"/>
   </r>
   <r>
     <x v="5"/>
     <x v="0"/>
-    <x v="25"/>
+    <n v="0.93400000000110595"/>
   </r>
   <r>
     <x v="5"/>
     <x v="0"/>
-    <x v="26"/>
+    <n v="0.69700000000011597"/>
   </r>
   <r>
     <x v="5"/>
     <x v="0"/>
-    <x v="27"/>
+    <n v="0.94800000000395801"/>
   </r>
   <r>
     <x v="5"/>
     <x v="0"/>
-    <x v="28"/>
+    <n v="0.77000000000407398"/>
   </r>
   <r>
     <x v="5"/>
     <x v="0"/>
-    <x v="29"/>
+    <n v="0.718999999997322"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
-    <x v="30"/>
+    <n v="0.42200000000047999"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
-    <x v="31"/>
+    <n v="0.50700000000142598"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
-    <x v="32"/>
+    <n v="0.37299999999959199"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
-    <x v="33"/>
+    <n v="0.44200000000091599"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
-    <x v="34"/>
+    <n v="0.39000000000305501"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="35"/>
+    <n v="0.49699999999938799"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="36"/>
+    <n v="0.48500000000058202"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="37"/>
+    <n v="0.57500000000072704"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="38"/>
+    <n v="0.50100000000020295"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="39"/>
+    <n v="0.49700000000302602"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
-    <x v="40"/>
+    <n v="0.92599999999947602"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
-    <x v="41"/>
+    <n v="1.0660000000032499"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
-    <x v="42"/>
+    <n v="1.0020000000003999"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
-    <x v="43"/>
+    <n v="0.64299999999639101"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
-    <x v="44"/>
+    <n v="0.90899999999964998"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
-    <x v="45"/>
+    <n v="0.78699999999662396"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
-    <x v="46"/>
+    <n v="0.74199999999836996"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
-    <x v="47"/>
+    <n v="0.76499999999941704"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
-    <x v="48"/>
+    <n v="0.98300000000017396"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
-    <x v="49"/>
+    <n v="0.84500000000116404"/>
   </r>
   <r>
     <x v="4"/>
     <x v="1"/>
-    <x v="50"/>
+    <n v="1.4489999999932399"/>
   </r>
   <r>
     <x v="4"/>
     <x v="1"/>
-    <x v="51"/>
+    <n v="0.82000000000698403"/>
   </r>
   <r>
     <x v="4"/>
     <x v="1"/>
-    <x v="52"/>
+    <n v="0.91000000000349202"/>
   </r>
   <r>
     <x v="4"/>
     <x v="1"/>
-    <x v="53"/>
+    <n v="1.21899999999732"/>
   </r>
   <r>
     <x v="4"/>
     <x v="1"/>
-    <x v="54"/>
+    <n v="1.11599999999452"/>
   </r>
   <r>
     <x v="5"/>
     <x v="1"/>
-    <x v="55"/>
+    <n v="0.888999999995576"/>
   </r>
   <r>
     <x v="5"/>
     <x v="1"/>
-    <x v="56"/>
+    <n v="1.0190000000002299"/>
   </r>
   <r>
     <x v="5"/>
     <x v="1"/>
-    <x v="57"/>
+    <n v="1.4089999999996501"/>
   </r>
   <r>
     <x v="5"/>
     <x v="1"/>
-    <x v="58"/>
+    <n v="1.47400000000197"/>
   </r>
   <r>
     <x v="5"/>
     <x v="1"/>
-    <x v="59"/>
+    <n v="1.0609999999869599"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0.42400000000270599"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0.47800000000279302"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0.40499999999883501"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0.43399999999382999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0.42399999999906801"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.54200000000128001"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.42900000000372501"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.47299999999813702"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.53499999999621595"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.58799999999609998"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0.59299999999347996"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0.60899999999674004"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0.62700000000768297"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0.463999999992665"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0.517000000007101"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="0.59500000000116404"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="0.72800000000279397"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="0.78500000000349202"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="0.81900000000314299"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="1.10300000000279"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1.0599999999976699"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="0.88399999999091905"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="0.85599999999976695"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1.1469999999972"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1.0650000000023201"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1.2690000000002299"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1.1780000000144299"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1.2650000000139601"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1.01399999999557"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1.18299999996088"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0.42200000000047999"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0.42799999999988297"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0.665000000000873"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0.56399999999848605"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0.48500000000058202"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.44000000000232797"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.472000000001571"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.50300000000061096"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.41700000000128001"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.46399999999994102"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0.546999999998661"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0.39699999999866098"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0.56500000000232797"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0.50400000000081402"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0.420000000001164"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.77500000000873104"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.74799999999231603"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.76499999999941704"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1.1080000000074499"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.79200000000128001"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1.4350000000122201"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1.34399999999732"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1.13300000000162"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1.1100000000005801"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1.00999999999476"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1.39600000000791"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="2.7630000000062802"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1.1710000000020899"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1.2660000000032501"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1.1880000000091899"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.44399999999950501"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.46700000000055297"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.42499999999927202"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.43699999999807898"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="0.50700000000142598"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.51899999999295598"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.42499999999563398"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.58299999999871899"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.37600000000384098"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.49599999999918498"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.69600000000355"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.70200000000477303"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.703000000001338"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.61100000000442301"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="0.54099999999743797"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="1.12400000000343"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="1.4530000000013299"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="0.84600000000500497"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="0.788000000000465"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="0.86399999998684496"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="1.16199999995296"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="1.2820000000065099"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="1.24900000001071"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="1.1330000000307301"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="1.33900000003632"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="1.6530000000056999"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="1.20999999999185"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="1.3739999999961501"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="1.6000000000058201"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="1.41700000001583"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A3:D11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField name="Total Connected Player" axis="axisRow" subtotalTop="0" showAll="0">
       <items count="7">
@@ -1887,78 +2617,17 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="Update Start Time" axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="3">
+    <pivotField name="Update Start Time" axis="axisCol" subtotalTop="0" showAll="0" sortType="ascending">
+      <items count="6">
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0">
-      <items count="61">
-        <item x="3"/>
-        <item x="4"/>
-        <item x="38"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="0"/>
-        <item x="36"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="10"/>
-        <item x="30"/>
-        <item x="6"/>
-        <item x="13"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="31"/>
-        <item x="12"/>
-        <item x="1"/>
-        <item x="39"/>
-        <item x="34"/>
-        <item x="19"/>
-        <item x="35"/>
-        <item x="44"/>
-        <item x="15"/>
-        <item x="37"/>
-        <item x="11"/>
-        <item x="23"/>
-        <item x="20"/>
-        <item x="18"/>
-        <item x="8"/>
-        <item x="43"/>
-        <item x="24"/>
-        <item x="21"/>
-        <item x="16"/>
-        <item x="40"/>
-        <item x="26"/>
-        <item x="17"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="29"/>
-        <item x="22"/>
-        <item x="14"/>
-        <item x="28"/>
-        <item x="48"/>
-        <item x="47"/>
-        <item x="49"/>
-        <item x="25"/>
-        <item x="27"/>
-        <item x="45"/>
-        <item x="53"/>
-        <item x="50"/>
-        <item x="56"/>
-        <item x="52"/>
-        <item x="51"/>
-        <item x="54"/>
-        <item x="57"/>
-        <item x="59"/>
-        <item x="46"/>
-        <item x="58"/>
-        <item x="55"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -1989,31 +2658,79 @@
   <colFields count="1">
     <field x="1"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="6">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Update Duration" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Sum of duration" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="1" format="0" series="1">
+  <chartFormats count="5">
+    <chartFormat chart="1" format="19" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="1" format="6" series="1">
+    <chartFormat chart="1" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="23" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2021,18 +2738,6 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -2051,8 +2756,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C61" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:C61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C151" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C151"/>
+  <sortState ref="A2:C151">
+    <sortCondition ref="B1:B151"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="players"/>
     <tableColumn id="2" name="starttime"/>
@@ -2063,15 +2771,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D13" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D31" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:D31"/>
+  <sortState ref="A2:D19">
+    <sortCondition ref="B1:B19"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="players"/>
     <tableColumn id="2" name="starttime"/>
-    <tableColumn id="3" name="durationaverage" dataDxfId="1">
+    <tableColumn id="3" name="durationaverage" dataDxfId="2">
       <calculatedColumnFormula>AVERAGEIFS(Table1[duration],Table1[players],A2,Table1[starttime],B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="durationstd" dataDxfId="0">
+    <tableColumn id="4" name="durationstd" dataDxfId="1">
       <calculatedColumnFormula array="1">_xlfn.STDEV.S(IF((Table1[players]=A2)*(Table1[starttime]=B2),Table1[duration]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2376,10 +3087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,10 +3446,10 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C32">
-        <v>0.44399999999950501</v>
+        <v>0.42200000000047999</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2746,10 +3457,10 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C33">
-        <v>0.46700000000055297</v>
+        <v>0.50700000000142598</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2757,10 +3468,10 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C34">
-        <v>0.42499999999927202</v>
+        <v>0.37299999999959199</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2768,10 +3479,10 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C35">
-        <v>0.43699999999807898</v>
+        <v>0.44200000000091599</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2779,10 +3490,10 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C36">
-        <v>0.50700000000142598</v>
+        <v>0.39000000000305501</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2790,10 +3501,10 @@
         <v>2</v>
       </c>
       <c r="B37">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C37">
-        <v>0.51899999999295598</v>
+        <v>0.49699999999938799</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2801,10 +3512,10 @@
         <v>2</v>
       </c>
       <c r="B38">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C38">
-        <v>0.42499999999563398</v>
+        <v>0.48500000000058202</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2812,10 +3523,10 @@
         <v>2</v>
       </c>
       <c r="B39">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C39">
-        <v>0.58299999999871899</v>
+        <v>0.57500000000072704</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2823,10 +3534,10 @@
         <v>2</v>
       </c>
       <c r="B40">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C40">
-        <v>0.37600000000384098</v>
+        <v>0.50100000000020295</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2834,10 +3545,10 @@
         <v>2</v>
       </c>
       <c r="B41">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C41">
-        <v>0.49599999999918498</v>
+        <v>0.49700000000302602</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2845,10 +3556,10 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C42">
-        <v>0.69600000000355</v>
+        <v>0.92599999999947602</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2856,10 +3567,10 @@
         <v>4</v>
       </c>
       <c r="B43">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C43">
-        <v>0.70200000000477303</v>
+        <v>1.0660000000032499</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2867,10 +3578,10 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C44">
-        <v>0.703000000001338</v>
+        <v>1.0020000000003999</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2878,10 +3589,10 @@
         <v>4</v>
       </c>
       <c r="B45">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C45">
-        <v>0.61100000000442301</v>
+        <v>0.64299999999639101</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2889,10 +3600,10 @@
         <v>4</v>
       </c>
       <c r="B46">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C46">
-        <v>0.54099999999743797</v>
+        <v>0.90899999999964998</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2900,10 +3611,10 @@
         <v>8</v>
       </c>
       <c r="B47">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C47">
-        <v>1.12400000000343</v>
+        <v>0.78699999999662396</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2911,10 +3622,10 @@
         <v>8</v>
       </c>
       <c r="B48">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C48">
-        <v>1.4530000000013299</v>
+        <v>0.74199999999836996</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2922,10 +3633,10 @@
         <v>8</v>
       </c>
       <c r="B49">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C49">
-        <v>0.84600000000500497</v>
+        <v>0.76499999999941704</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2933,10 +3644,10 @@
         <v>8</v>
       </c>
       <c r="B50">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C50">
-        <v>0.788000000000465</v>
+        <v>0.98300000000017396</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2944,10 +3655,10 @@
         <v>8</v>
       </c>
       <c r="B51">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C51">
-        <v>0.86399999998684496</v>
+        <v>0.84500000000116404</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2955,10 +3666,10 @@
         <v>12</v>
       </c>
       <c r="B52">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C52">
-        <v>1.16199999995296</v>
+        <v>1.4489999999932399</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2966,10 +3677,10 @@
         <v>12</v>
       </c>
       <c r="B53">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C53">
-        <v>1.2820000000065099</v>
+        <v>0.82000000000698403</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2977,10 +3688,10 @@
         <v>12</v>
       </c>
       <c r="B54">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C54">
-        <v>1.24900000001071</v>
+        <v>0.91000000000349202</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2988,10 +3699,10 @@
         <v>12</v>
       </c>
       <c r="B55">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C55">
-        <v>1.1330000000307301</v>
+        <v>1.21899999999732</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2999,10 +3710,10 @@
         <v>12</v>
       </c>
       <c r="B56">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C56">
-        <v>1.33900000003632</v>
+        <v>1.11599999999452</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3010,10 +3721,10 @@
         <v>16</v>
       </c>
       <c r="B57">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C57">
-        <v>1.6530000000056999</v>
+        <v>0.888999999995576</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3021,10 +3732,10 @@
         <v>16</v>
       </c>
       <c r="B58">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C58">
-        <v>1.20999999999185</v>
+        <v>1.0190000000002299</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3032,10 +3743,10 @@
         <v>16</v>
       </c>
       <c r="B59">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C59">
-        <v>1.3739999999961501</v>
+        <v>1.4089999999996501</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3043,10 +3754,10 @@
         <v>16</v>
       </c>
       <c r="B60">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="C60">
-        <v>1.6000000000058201</v>
+        <v>1.47400000000197</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3054,9 +3765,999 @@
         <v>16</v>
       </c>
       <c r="B61">
+        <v>250</v>
+      </c>
+      <c r="C61">
+        <v>1.0609999999869599</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>500</v>
+      </c>
+      <c r="C62">
+        <v>0.42400000000270599</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>500</v>
+      </c>
+      <c r="C63">
+        <v>0.47800000000279302</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>500</v>
+      </c>
+      <c r="C64">
+        <v>0.40499999999883501</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>500</v>
+      </c>
+      <c r="C65">
+        <v>0.43399999999382999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>500</v>
+      </c>
+      <c r="C66">
+        <v>0.42399999999906801</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67">
+        <v>500</v>
+      </c>
+      <c r="C67">
+        <v>0.54200000000128001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68">
+        <v>500</v>
+      </c>
+      <c r="C68">
+        <v>0.42900000000372501</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69">
+        <v>500</v>
+      </c>
+      <c r="C69">
+        <v>0.47299999999813702</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>500</v>
+      </c>
+      <c r="C70">
+        <v>0.53499999999621595</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71">
+        <v>500</v>
+      </c>
+      <c r="C71">
+        <v>0.58799999999609998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>4</v>
+      </c>
+      <c r="B72">
+        <v>500</v>
+      </c>
+      <c r="C72">
+        <v>0.59299999999347996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>4</v>
+      </c>
+      <c r="B73">
+        <v>500</v>
+      </c>
+      <c r="C73">
+        <v>0.60899999999674004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>4</v>
+      </c>
+      <c r="B74">
+        <v>500</v>
+      </c>
+      <c r="C74">
+        <v>0.62700000000768297</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="B75">
+        <v>500</v>
+      </c>
+      <c r="C75">
+        <v>0.463999999992665</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>4</v>
+      </c>
+      <c r="B76">
+        <v>500</v>
+      </c>
+      <c r="C76">
+        <v>0.517000000007101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>8</v>
+      </c>
+      <c r="B77">
+        <v>500</v>
+      </c>
+      <c r="C77">
+        <v>0.59500000000116404</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>8</v>
+      </c>
+      <c r="B78">
+        <v>500</v>
+      </c>
+      <c r="C78">
+        <v>0.72800000000279397</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>8</v>
+      </c>
+      <c r="B79">
+        <v>500</v>
+      </c>
+      <c r="C79">
+        <v>0.78500000000349202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>8</v>
+      </c>
+      <c r="B80">
+        <v>500</v>
+      </c>
+      <c r="C80">
+        <v>0.81900000000314299</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>8</v>
+      </c>
+      <c r="B81">
+        <v>500</v>
+      </c>
+      <c r="C81">
+        <v>1.10300000000279</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>12</v>
+      </c>
+      <c r="B82">
+        <v>500</v>
+      </c>
+      <c r="C82">
+        <v>1.0599999999976699</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>12</v>
+      </c>
+      <c r="B83">
+        <v>500</v>
+      </c>
+      <c r="C83">
+        <v>0.88399999999091905</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>12</v>
+      </c>
+      <c r="B84">
+        <v>500</v>
+      </c>
+      <c r="C84">
+        <v>0.85599999999976695</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>12</v>
+      </c>
+      <c r="B85">
+        <v>500</v>
+      </c>
+      <c r="C85">
+        <v>1.1469999999972</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>12</v>
+      </c>
+      <c r="B86">
+        <v>500</v>
+      </c>
+      <c r="C86">
+        <v>1.0650000000023201</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>16</v>
+      </c>
+      <c r="B87">
+        <v>500</v>
+      </c>
+      <c r="C87">
+        <v>1.2690000000002299</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>16</v>
+      </c>
+      <c r="B88">
+        <v>500</v>
+      </c>
+      <c r="C88">
+        <v>1.1780000000144299</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>16</v>
+      </c>
+      <c r="B89">
+        <v>500</v>
+      </c>
+      <c r="C89">
+        <v>1.2650000000139601</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>16</v>
+      </c>
+      <c r="B90">
+        <v>500</v>
+      </c>
+      <c r="C90">
+        <v>1.01399999999557</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>16</v>
+      </c>
+      <c r="B91">
+        <v>500</v>
+      </c>
+      <c r="C91">
+        <v>1.18299999996088</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>750</v>
+      </c>
+      <c r="C92">
+        <v>0.42200000000047999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>750</v>
+      </c>
+      <c r="C93">
+        <v>0.42799999999988297</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94">
+        <v>750</v>
+      </c>
+      <c r="C94">
+        <v>0.665000000000873</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>750</v>
+      </c>
+      <c r="C95">
+        <v>0.56399999999848605</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1</v>
+      </c>
+      <c r="B96">
+        <v>750</v>
+      </c>
+      <c r="C96">
+        <v>0.48500000000058202</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2</v>
+      </c>
+      <c r="B97">
+        <v>750</v>
+      </c>
+      <c r="C97">
+        <v>0.44000000000232797</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>750</v>
+      </c>
+      <c r="C98">
+        <v>0.472000000001571</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99">
+        <v>750</v>
+      </c>
+      <c r="C99">
+        <v>0.50300000000061096</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100">
+        <v>750</v>
+      </c>
+      <c r="C100">
+        <v>0.41700000000128001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="B101">
+        <v>750</v>
+      </c>
+      <c r="C101">
+        <v>0.46399999999994102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <v>750</v>
+      </c>
+      <c r="C102">
+        <v>0.546999999998661</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <v>750</v>
+      </c>
+      <c r="C103">
+        <v>0.39699999999866098</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>750</v>
+      </c>
+      <c r="C104">
+        <v>0.56500000000232797</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>4</v>
+      </c>
+      <c r="B105">
+        <v>750</v>
+      </c>
+      <c r="C105">
+        <v>0.50400000000081402</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>750</v>
+      </c>
+      <c r="C106">
+        <v>0.420000000001164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>8</v>
+      </c>
+      <c r="B107">
+        <v>750</v>
+      </c>
+      <c r="C107">
+        <v>0.77500000000873104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>8</v>
+      </c>
+      <c r="B108">
+        <v>750</v>
+      </c>
+      <c r="C108">
+        <v>0.74799999999231603</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>8</v>
+      </c>
+      <c r="B109">
+        <v>750</v>
+      </c>
+      <c r="C109">
+        <v>0.76499999999941704</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>8</v>
+      </c>
+      <c r="B110">
+        <v>750</v>
+      </c>
+      <c r="C110">
+        <v>1.1080000000074499</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>8</v>
+      </c>
+      <c r="B111">
+        <v>750</v>
+      </c>
+      <c r="C111">
+        <v>0.79200000000128001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>12</v>
+      </c>
+      <c r="B112">
+        <v>750</v>
+      </c>
+      <c r="C112">
+        <v>1.4350000000122201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>12</v>
+      </c>
+      <c r="B113">
+        <v>750</v>
+      </c>
+      <c r="C113">
+        <v>1.34399999999732</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>12</v>
+      </c>
+      <c r="B114">
+        <v>750</v>
+      </c>
+      <c r="C114">
+        <v>1.13300000000162</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>12</v>
+      </c>
+      <c r="B115">
+        <v>750</v>
+      </c>
+      <c r="C115">
+        <v>1.1100000000005801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>12</v>
+      </c>
+      <c r="B116">
+        <v>750</v>
+      </c>
+      <c r="C116">
+        <v>1.00999999999476</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>16</v>
+      </c>
+      <c r="B117">
+        <v>750</v>
+      </c>
+      <c r="C117">
+        <v>1.39600000000791</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>16</v>
+      </c>
+      <c r="B118">
+        <v>750</v>
+      </c>
+      <c r="C118">
+        <v>2.7630000000062802</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>16</v>
+      </c>
+      <c r="B119">
+        <v>750</v>
+      </c>
+      <c r="C119">
+        <v>1.1710000000020899</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>16</v>
+      </c>
+      <c r="B120">
+        <v>750</v>
+      </c>
+      <c r="C120">
+        <v>1.2660000000032501</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>16</v>
+      </c>
+      <c r="B121">
+        <v>750</v>
+      </c>
+      <c r="C121">
+        <v>1.1880000000091899</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122">
         <v>1000</v>
       </c>
-      <c r="C61">
+      <c r="C122">
+        <v>0.44399999999950501</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1</v>
+      </c>
+      <c r="B123">
+        <v>1000</v>
+      </c>
+      <c r="C123">
+        <v>0.46700000000055297</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124">
+        <v>1000</v>
+      </c>
+      <c r="C124">
+        <v>0.42499999999927202</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>1</v>
+      </c>
+      <c r="B125">
+        <v>1000</v>
+      </c>
+      <c r="C125">
+        <v>0.43699999999807898</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>1000</v>
+      </c>
+      <c r="C126">
+        <v>0.50700000000142598</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2</v>
+      </c>
+      <c r="B127">
+        <v>1000</v>
+      </c>
+      <c r="C127">
+        <v>0.51899999999295598</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>2</v>
+      </c>
+      <c r="B128">
+        <v>1000</v>
+      </c>
+      <c r="C128">
+        <v>0.42499999999563398</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>2</v>
+      </c>
+      <c r="B129">
+        <v>1000</v>
+      </c>
+      <c r="C129">
+        <v>0.58299999999871899</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>2</v>
+      </c>
+      <c r="B130">
+        <v>1000</v>
+      </c>
+      <c r="C130">
+        <v>0.37600000000384098</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>2</v>
+      </c>
+      <c r="B131">
+        <v>1000</v>
+      </c>
+      <c r="C131">
+        <v>0.49599999999918498</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>4</v>
+      </c>
+      <c r="B132">
+        <v>1000</v>
+      </c>
+      <c r="C132">
+        <v>0.69600000000355</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>4</v>
+      </c>
+      <c r="B133">
+        <v>1000</v>
+      </c>
+      <c r="C133">
+        <v>0.70200000000477303</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>4</v>
+      </c>
+      <c r="B134">
+        <v>1000</v>
+      </c>
+      <c r="C134">
+        <v>0.703000000001338</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>4</v>
+      </c>
+      <c r="B135">
+        <v>1000</v>
+      </c>
+      <c r="C135">
+        <v>0.61100000000442301</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>4</v>
+      </c>
+      <c r="B136">
+        <v>1000</v>
+      </c>
+      <c r="C136">
+        <v>0.54099999999743797</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>8</v>
+      </c>
+      <c r="B137">
+        <v>1000</v>
+      </c>
+      <c r="C137">
+        <v>1.12400000000343</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>8</v>
+      </c>
+      <c r="B138">
+        <v>1000</v>
+      </c>
+      <c r="C138">
+        <v>1.4530000000013299</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>8</v>
+      </c>
+      <c r="B139">
+        <v>1000</v>
+      </c>
+      <c r="C139">
+        <v>0.84600000000500497</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>8</v>
+      </c>
+      <c r="B140">
+        <v>1000</v>
+      </c>
+      <c r="C140">
+        <v>0.788000000000465</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>8</v>
+      </c>
+      <c r="B141">
+        <v>1000</v>
+      </c>
+      <c r="C141">
+        <v>0.86399999998684496</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>12</v>
+      </c>
+      <c r="B142">
+        <v>1000</v>
+      </c>
+      <c r="C142">
+        <v>1.16199999995296</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>12</v>
+      </c>
+      <c r="B143">
+        <v>1000</v>
+      </c>
+      <c r="C143">
+        <v>1.2820000000065099</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>12</v>
+      </c>
+      <c r="B144">
+        <v>1000</v>
+      </c>
+      <c r="C144">
+        <v>1.24900000001071</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>12</v>
+      </c>
+      <c r="B145">
+        <v>1000</v>
+      </c>
+      <c r="C145">
+        <v>1.1330000000307301</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>12</v>
+      </c>
+      <c r="B146">
+        <v>1000</v>
+      </c>
+      <c r="C146">
+        <v>1.33900000003632</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>16</v>
+      </c>
+      <c r="B147">
+        <v>1000</v>
+      </c>
+      <c r="C147">
+        <v>1.6530000000056999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>16</v>
+      </c>
+      <c r="B148">
+        <v>1000</v>
+      </c>
+      <c r="C148">
+        <v>1.20999999999185</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>16</v>
+      </c>
+      <c r="B149">
+        <v>1000</v>
+      </c>
+      <c r="C149">
+        <v>1.3739999999961501</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>16</v>
+      </c>
+      <c r="B150">
+        <v>1000</v>
+      </c>
+      <c r="C150">
+        <v>1.6000000000058201</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>16</v>
+      </c>
+      <c r="B151">
+        <v>1000</v>
+      </c>
+      <c r="C151">
         <v>1.41700000001583</v>
       </c>
     </row>
@@ -3071,10 +4772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,15 +4901,15 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>1000</v>
-      </c>
-      <c r="C8">
+        <v>500</v>
+      </c>
+      <c r="C8" s="2">
         <f>AVERAGEIFS(Table1[duration],Table1[players],A8,Table1[starttime],B8)</f>
-        <v>0.45599999999976698</v>
-      </c>
-      <c r="D8">
+        <v>0.43299999999944638</v>
+      </c>
+      <c r="D8" s="2">
         <f t="array" ref="D8">_xlfn.STDEV.S(IF((Table1[players]=A8)*(Table1[starttime]=B8),Table1[duration]))</f>
-        <v>3.2357379375838012E-2</v>
+        <v>2.7258026342126918E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3216,15 +4917,15 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>1000</v>
-      </c>
-      <c r="C9">
+        <v>500</v>
+      </c>
+      <c r="C9" s="2">
         <f>AVERAGEIFS(Table1[duration],Table1[players],A9,Table1[starttime],B9)</f>
-        <v>0.47979999999806699</v>
-      </c>
-      <c r="D9">
+        <v>0.51339999999909158</v>
+      </c>
+      <c r="D9" s="2">
         <f t="array" ref="D9">_xlfn.STDEV.S(IF((Table1[players]=A9)*(Table1[starttime]=B9),Table1[duration]))</f>
-        <v>8.0973452437879512E-2</v>
+        <v>6.2460387444462695E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3232,15 +4933,15 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10">
+        <v>500</v>
+      </c>
+      <c r="C10" s="2">
         <f>AVERAGEIFS(Table1[duration],Table1[players],A10,Table1[starttime],B10)</f>
-        <v>0.65060000000230445</v>
-      </c>
-      <c r="D10">
+        <v>0.56199999999953376</v>
+      </c>
+      <c r="D10" s="2">
         <f t="array" ref="D10">_xlfn.STDEV.S(IF((Table1[players]=A10)*(Table1[starttime]=B10),Table1[duration]))</f>
-        <v>7.2507241019715618E-2</v>
+        <v>6.8963758600236208E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3248,15 +4949,15 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1000</v>
-      </c>
-      <c r="C11">
+        <v>500</v>
+      </c>
+      <c r="C11" s="2">
         <f>AVERAGEIFS(Table1[duration],Table1[players],A11,Table1[starttime],B11)</f>
-        <v>1.0149999999994148</v>
-      </c>
-      <c r="D11">
+        <v>0.80600000000267646</v>
+      </c>
+      <c r="D11" s="2">
         <f t="array" ref="D11">_xlfn.STDEV.S(IF((Table1[players]=A11)*(Table1[starttime]=B11),Table1[duration]))</f>
-        <v>0.27686458784213608</v>
+        <v>0.18669761648228511</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,15 +4965,15 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1000</v>
-      </c>
-      <c r="C12">
+        <v>500</v>
+      </c>
+      <c r="C12" s="2">
         <f>AVERAGEIFS(Table1[duration],Table1[players],A12,Table1[starttime],B12)</f>
-        <v>1.2330000000074459</v>
-      </c>
-      <c r="D12">
+        <v>1.0023999999975752</v>
+      </c>
+      <c r="D12" s="2">
         <f t="array" ref="D12">_xlfn.STDEV.S(IF((Table1[players]=A12)*(Table1[starttime]=B12),Table1[duration]))</f>
-        <v>8.5049985316304144E-2</v>
+        <v>0.126092426419503</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3280,15 +4981,303 @@
         <v>16</v>
       </c>
       <c r="B13">
+        <v>500</v>
+      </c>
+      <c r="C13" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A13,Table1[starttime],B13)</f>
+        <v>1.1817999999970139</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="array" ref="D13">_xlfn.STDEV.S(IF((Table1[players]=A13)*(Table1[starttime]=B13),Table1[duration]))</f>
+        <v>0.10331843979131486</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>1000</v>
       </c>
-      <c r="C13">
-        <f>AVERAGEIFS(Table1[duration],Table1[players],A13,Table1[starttime],B13)</f>
+      <c r="C14">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A14,Table1[starttime],B14)</f>
+        <v>0.45599999999976698</v>
+      </c>
+      <c r="D14">
+        <f t="array" ref="D14">_xlfn.STDEV.S(IF((Table1[players]=A14)*(Table1[starttime]=B14),Table1[duration]))</f>
+        <v>3.2357379375838012E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A15,Table1[starttime],B15)</f>
+        <v>0.47979999999806699</v>
+      </c>
+      <c r="D15">
+        <f t="array" ref="D15">_xlfn.STDEV.S(IF((Table1[players]=A15)*(Table1[starttime]=B15),Table1[duration]))</f>
+        <v>8.0973452437879512E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>1000</v>
+      </c>
+      <c r="C16">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A16,Table1[starttime],B16)</f>
+        <v>0.65060000000230445</v>
+      </c>
+      <c r="D16">
+        <f t="array" ref="D16">_xlfn.STDEV.S(IF((Table1[players]=A16)*(Table1[starttime]=B16),Table1[duration]))</f>
+        <v>7.2507241019715618E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>1000</v>
+      </c>
+      <c r="C17">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A17,Table1[starttime],B17)</f>
+        <v>1.0149999999994148</v>
+      </c>
+      <c r="D17">
+        <f t="array" ref="D17">_xlfn.STDEV.S(IF((Table1[players]=A17)*(Table1[starttime]=B17),Table1[duration]))</f>
+        <v>0.27686458784213608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>1000</v>
+      </c>
+      <c r="C18">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A18,Table1[starttime],B18)</f>
+        <v>1.2330000000074459</v>
+      </c>
+      <c r="D18">
+        <f t="array" ref="D18">_xlfn.STDEV.S(IF((Table1[players]=A18)*(Table1[starttime]=B18),Table1[duration]))</f>
+        <v>8.5049985316304144E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>1000</v>
+      </c>
+      <c r="C19">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A19,Table1[starttime],B19)</f>
         <v>1.4508000000030701</v>
       </c>
-      <c r="D13">
-        <f t="array" ref="D13">_xlfn.STDEV.S(IF((Table1[players]=A13)*(Table1[starttime]=B13),Table1[duration]))</f>
+      <c r="D19">
+        <f t="array" ref="D19">_xlfn.STDEV.S(IF((Table1[players]=A19)*(Table1[starttime]=B19),Table1[duration]))</f>
         <v>0.17900474854559625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>250</v>
+      </c>
+      <c r="C20" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A20,Table1[starttime],B20)</f>
+        <v>0.42680000000109375</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="array" ref="D20">_xlfn.STDEV.S(IF((Table1[players]=A20)*(Table1[starttime]=B20),Table1[duration]))</f>
+        <v>5.2284797025691866E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>250</v>
+      </c>
+      <c r="C21" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A21,Table1[starttime],B21)</f>
+        <v>0.51100000000078516</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="array" ref="D21">_xlfn.STDEV.S(IF((Table1[players]=A21)*(Table1[starttime]=B21),Table1[duration]))</f>
+        <v>3.6276714294403593E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>250</v>
+      </c>
+      <c r="C22" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A22,Table1[starttime],B22)</f>
+        <v>0.90919999999983347</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="array" ref="D22">_xlfn.STDEV.S(IF((Table1[players]=A22)*(Table1[starttime]=B22),Table1[duration]))</f>
+        <v>0.16151068076368597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>250</v>
+      </c>
+      <c r="C23" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A23,Table1[starttime],B23)</f>
+        <v>0.82439999999914981</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="array" ref="D23">_xlfn.STDEV.S(IF((Table1[players]=A23)*(Table1[starttime]=B23),Table1[duration]))</f>
+        <v>9.6559826015654202E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>250</v>
+      </c>
+      <c r="C24" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A24,Table1[starttime],B24)</f>
+        <v>1.1027999999991114</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="array" ref="D24">_xlfn.STDEV.S(IF((Table1[players]=A24)*(Table1[starttime]=B24),Table1[duration]))</f>
+        <v>0.25033916992215488</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <v>250</v>
+      </c>
+      <c r="C25" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A25,Table1[starttime],B25)</f>
+        <v>1.1703999999968773</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="array" ref="D25">_xlfn.STDEV.S(IF((Table1[players]=A25)*(Table1[starttime]=B25),Table1[duration]))</f>
+        <v>0.25650497071514144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>750</v>
+      </c>
+      <c r="C26" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A26,Table1[starttime],B26)</f>
+        <v>0.51280000000006087</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="array" ref="D26">_xlfn.STDEV.S(IF((Table1[players]=A26)*(Table1[starttime]=B26),Table1[duration]))</f>
+        <v>0.102463164112781</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>750</v>
+      </c>
+      <c r="C27" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A27,Table1[starttime],B27)</f>
+        <v>0.45920000000114614</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="array" ref="D27">_xlfn.STDEV.S(IF((Table1[players]=A27)*(Table1[starttime]=B27),Table1[duration]))</f>
+        <v>3.2614413990963195E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>750</v>
+      </c>
+      <c r="C28" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A28,Table1[starttime],B28)</f>
+        <v>0.48660000000032555</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="array" ref="D28">_xlfn.STDEV.S(IF((Table1[players]=A28)*(Table1[starttime]=B28),Table1[duration]))</f>
+        <v>7.5101930734696468E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>750</v>
+      </c>
+      <c r="C29" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A29,Table1[starttime],B29)</f>
+        <v>0.83760000000183865</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="array" ref="D29">_xlfn.STDEV.S(IF((Table1[players]=A29)*(Table1[starttime]=B29),Table1[duration]))</f>
+        <v>0.15199769735450114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>750</v>
+      </c>
+      <c r="C30" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A30,Table1[starttime],B30)</f>
+        <v>1.2064000000013</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="array" ref="D30">_xlfn.STDEV.S(IF((Table1[players]=A30)*(Table1[starttime]=B30),Table1[duration]))</f>
+        <v>0.1763839561911453</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>750</v>
+      </c>
+      <c r="C31" s="2">
+        <f>AVERAGEIFS(Table1[duration],Table1[players],A31,Table1[starttime],B31)</f>
+        <v>1.556800000005744</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="array" ref="D31">_xlfn.STDEV.S(IF((Table1[players]=A31)*(Table1[starttime]=B31),Table1[duration]))</f>
+        <v>0.68010932944680402</v>
       </c>
     </row>
   </sheetData>
@@ -3301,20 +5290,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D11"/>
+  <dimension ref="A3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="3" max="4" width="7" customWidth="1"/>
+    <col min="5" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" customWidth="1"/>
     <col min="10" max="11" width="7" customWidth="1"/>
@@ -3393,7 +5381,7 @@
     <col min="122" max="122" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3401,7 +5389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3409,108 +5397,180 @@
         <v>0</v>
       </c>
       <c r="C4">
+        <v>250</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+      <c r="E4">
+        <v>750</v>
+      </c>
+      <c r="F4">
         <v>1000</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>0.39859999999607643</v>
+        <v>1.992999999980382</v>
       </c>
       <c r="C5" s="2">
-        <v>0.45599999999976698</v>
+        <v>2.1340000000054689</v>
       </c>
       <c r="D5" s="2">
-        <v>0.42729999999792173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.164999999997232</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.5640000000003043</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.279999999998835</v>
+      </c>
+      <c r="G5" s="2">
+        <v>11.135999999982221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
       <c r="B6" s="2">
-        <v>0.48080000000190859</v>
+        <v>2.4040000000095429</v>
       </c>
       <c r="C6" s="2">
-        <v>0.47979999999806699</v>
+        <v>2.5550000000039259</v>
       </c>
       <c r="D6" s="2">
-        <v>0.48029999999998785</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.566999999995458</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.2960000000057308</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.3989999999903349</v>
+      </c>
+      <c r="G6" s="2">
+        <v>12.221000000004992</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>0.54400000000023252</v>
+        <v>2.7200000000011624</v>
       </c>
       <c r="C7" s="2">
-        <v>0.65060000000230445</v>
+        <v>4.5459999999991672</v>
       </c>
       <c r="D7" s="2">
-        <v>0.59730000000126837</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.809999999997669</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.4330000000016279</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3.253000000011522</v>
+      </c>
+      <c r="G7" s="2">
+        <v>15.762000000011149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>0.61200000000026145</v>
+        <v>3.060000000001307</v>
       </c>
       <c r="C8" s="2">
-        <v>1.0149999999994148</v>
+        <v>4.1219999999957491</v>
       </c>
       <c r="D8" s="2">
-        <v>0.81349999999983813</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.0300000000133824</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.1880000000091933</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.0749999999970745</v>
+      </c>
+      <c r="G8" s="2">
+        <v>20.475000000016706</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>0.63680000000022063</v>
+        <v>3.1840000000011033</v>
       </c>
       <c r="C9" s="2">
-        <v>1.2330000000074459</v>
+        <v>5.5139999999955567</v>
       </c>
       <c r="D9" s="2">
-        <v>0.93490000000383344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.0119999999878759</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6.0320000000064997</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6.1650000000372298</v>
+      </c>
+      <c r="G9" s="2">
+        <v>25.907000000028269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>0.81360000000131516</v>
+        <v>4.0680000000065757</v>
       </c>
       <c r="C10" s="2">
-        <v>1.4508000000030701</v>
+        <v>5.8519999999843861</v>
       </c>
       <c r="D10" s="2">
-        <v>1.1322000000021926</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.9089999999850695</v>
+      </c>
+      <c r="E10" s="2">
+        <v>7.7840000000287199</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7.2540000000153499</v>
+      </c>
+      <c r="G10" s="2">
+        <v>30.867000000020099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2">
-        <v>0.58096666666666918</v>
+        <v>17.429000000000073</v>
       </c>
       <c r="C11" s="2">
-        <v>0.88086666666834501</v>
+        <v>24.722999999984253</v>
       </c>
       <c r="D11" s="2">
-        <v>0.7309166666675071</v>
+        <v>22.492999999976686</v>
+      </c>
+      <c r="E11" s="2">
+        <v>25.297000000052073</v>
+      </c>
+      <c r="F11" s="2">
+        <v>26.426000000050347</v>
+      </c>
+      <c r="G11" s="2">
+        <v>116.36800000006345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>